<commit_message>
changes to parts and regenrated
</commit_message>
<xml_diff>
--- a/Project Outputs for USB-SMB-ISO-CP2112/Manufacturing Data/BOM/Bill of Materials-USB-SMB-ISO-CP2112.xlsx
+++ b/Project Outputs for USB-SMB-ISO-CP2112/Manufacturing Data/BOM/Bill of Materials-USB-SMB-ISO-CP2112.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\desktop\Documents\Project Files\Altium\Projects\Project - Devlopment\USB-SMB-ISO-CP2112\Project Outputs for USB-SMB-ISO-CP2112\Manufacturing Data\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0E221910-D3CC-4C9D-92F8-166C64CA3C05}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{53298405-E817-4555-98CD-E3E9C46ABEA7}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14310" windowHeight="13290" xr2:uid="{BCACB02E-CA96-430D-BD09-9E3108DAB177}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14310" windowHeight="13290" xr2:uid="{844A3B0B-1A98-43A2-BA39-CE53BDBBC7FA}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-USB-SMB-ISO-C" sheetId="1" r:id="rId1"/>
@@ -860,7 +860,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{331D785A-3E60-43BF-A283-4784108940C6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AE961C3-B15A-4AEC-990B-20FEC8D9CFA0}">
   <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>